<commit_message>
[Iteration 37] - [Amit] Client specific installer settings
This check in has the following changes:
1. The client specific DB configuration files.
2. Created GSTR 1 JSON file
3. Fixes issues with URL at register and store opening
4. Showing and hiding sale screen components.
5. Updated the length for phone no to 15 in customer screens
</commit_message>
<xml_diff>
--- a/reference/gst_state_codes.xlsx
+++ b/reference/gst_state_codes.xlsx
@@ -4,17 +4,18 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="GST STATES" sheetId="1" r:id="rId1"/>
+    <sheet name="UOM" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="559" uniqueCount="186">
   <si>
     <t>Sr. No.</t>
   </si>
@@ -293,13 +294,292 @@
   </si>
   <si>
     <t>'));</t>
+  </si>
+  <si>
+    <t>BAG</t>
+  </si>
+  <si>
+    <t>BAGS</t>
+  </si>
+  <si>
+    <t>QTY</t>
+  </si>
+  <si>
+    <t>INSERT INTO `pi_pos_industry`.`uom_master` (`name`, `code`, `description`, `type`, `is_primary`, `created_by`, `created_date`)</t>
+  </si>
+  <si>
+    <t>BAL</t>
+  </si>
+  <si>
+    <t>BALE</t>
+  </si>
+  <si>
+    <t>BDL</t>
+  </si>
+  <si>
+    <t>BUNDLES</t>
+  </si>
+  <si>
+    <t>BKL</t>
+  </si>
+  <si>
+    <t>BUCKLES</t>
+  </si>
+  <si>
+    <t>BOU</t>
+  </si>
+  <si>
+    <t>BILLION OF UNITS</t>
+  </si>
+  <si>
+    <t>BOX</t>
+  </si>
+  <si>
+    <t>BTL</t>
+  </si>
+  <si>
+    <t>BOTTLES</t>
+  </si>
+  <si>
+    <t>BUN</t>
+  </si>
+  <si>
+    <t>BUNCHES</t>
+  </si>
+  <si>
+    <t>CAN</t>
+  </si>
+  <si>
+    <t>CANS</t>
+  </si>
+  <si>
+    <t>CBM</t>
+  </si>
+  <si>
+    <t>CUBIC METERS</t>
+  </si>
+  <si>
+    <t>VOLUME</t>
+  </si>
+  <si>
+    <t>CCM</t>
+  </si>
+  <si>
+    <t>CUBIC CENTIMETERS</t>
+  </si>
+  <si>
+    <t>CMS</t>
+  </si>
+  <si>
+    <t>CENTIMETERS</t>
+  </si>
+  <si>
+    <t>LENGTH</t>
+  </si>
+  <si>
+    <t>CTN</t>
+  </si>
+  <si>
+    <t>CARTONS</t>
+  </si>
+  <si>
+    <t>DOZ</t>
+  </si>
+  <si>
+    <t>DOZENS</t>
+  </si>
+  <si>
+    <t>DRM</t>
+  </si>
+  <si>
+    <t>DRUMS</t>
+  </si>
+  <si>
+    <t>GGK</t>
+  </si>
+  <si>
+    <t>GREAT GROSS</t>
+  </si>
+  <si>
+    <t>GMS</t>
+  </si>
+  <si>
+    <t>GRAMMES</t>
+  </si>
+  <si>
+    <t>WEIGHT</t>
+  </si>
+  <si>
+    <t>GRS</t>
+  </si>
+  <si>
+    <t>GROSS</t>
+  </si>
+  <si>
+    <t>GYD</t>
+  </si>
+  <si>
+    <t>GROSS YARDS</t>
+  </si>
+  <si>
+    <t>KGS</t>
+  </si>
+  <si>
+    <t>KILOGRAMS</t>
+  </si>
+  <si>
+    <t>KLR</t>
+  </si>
+  <si>
+    <t>KILOLITRE</t>
+  </si>
+  <si>
+    <t>KME</t>
+  </si>
+  <si>
+    <t>KILOMETRE</t>
+  </si>
+  <si>
+    <t>MLT</t>
+  </si>
+  <si>
+    <t>MILILITRE</t>
+  </si>
+  <si>
+    <t>MTR</t>
+  </si>
+  <si>
+    <t>METERS</t>
+  </si>
+  <si>
+    <t>MTS</t>
+  </si>
+  <si>
+    <t>METRIC TON</t>
+  </si>
+  <si>
+    <t>NOS</t>
+  </si>
+  <si>
+    <t>NUMBERS</t>
+  </si>
+  <si>
+    <t>PAC</t>
+  </si>
+  <si>
+    <t>PACKS</t>
+  </si>
+  <si>
+    <t>PCS</t>
+  </si>
+  <si>
+    <t>PIECES</t>
+  </si>
+  <si>
+    <t>PRS</t>
+  </si>
+  <si>
+    <t>PAIRS</t>
+  </si>
+  <si>
+    <t>QTL</t>
+  </si>
+  <si>
+    <t>QUINTAL</t>
+  </si>
+  <si>
+    <t>ROL</t>
+  </si>
+  <si>
+    <t>ROLLS</t>
+  </si>
+  <si>
+    <t>SET</t>
+  </si>
+  <si>
+    <t>SETS</t>
+  </si>
+  <si>
+    <t>SQF</t>
+  </si>
+  <si>
+    <t>SQUARE FEET</t>
+  </si>
+  <si>
+    <t>AREA</t>
+  </si>
+  <si>
+    <t>SQM</t>
+  </si>
+  <si>
+    <t>SQUARE METERS</t>
+  </si>
+  <si>
+    <t>SQY</t>
+  </si>
+  <si>
+    <t>SQUARE YARDS</t>
+  </si>
+  <si>
+    <t>TBS</t>
+  </si>
+  <si>
+    <t>TABLETS</t>
+  </si>
+  <si>
+    <t>TGM</t>
+  </si>
+  <si>
+    <t>TEN GROSS</t>
+  </si>
+  <si>
+    <t>THD</t>
+  </si>
+  <si>
+    <t>THOUSANDS</t>
+  </si>
+  <si>
+    <t>TON</t>
+  </si>
+  <si>
+    <t>TONNES</t>
+  </si>
+  <si>
+    <t>TUB</t>
+  </si>
+  <si>
+    <t>TUBES</t>
+  </si>
+  <si>
+    <t>UGS</t>
+  </si>
+  <si>
+    <t>US GALLONS</t>
+  </si>
+  <si>
+    <t>UNT</t>
+  </si>
+  <si>
+    <t>UNITS</t>
+  </si>
+  <si>
+    <t>YDS</t>
+  </si>
+  <si>
+    <t>YARDS</t>
+  </si>
+  <si>
+    <t>OTH</t>
+  </si>
+  <si>
+    <t>OTHERS</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -319,6 +599,12 @@
       <color rgb="FF222222"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="4">
@@ -341,7 +627,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -364,11 +650,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -385,6 +686,9 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -691,8 +995,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2:R38"/>
+    <sheetView topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="C48" sqref="C48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2582,4 +2886,946 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G44"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="B18" workbookViewId="0">
+      <selection activeCell="F27" sqref="F27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="6" max="6" width="114.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="B1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C1" t="s">
+        <v>95</v>
+      </c>
+      <c r="D1">
+        <v>0</v>
+      </c>
+      <c r="F1" t="s">
+        <v>96</v>
+      </c>
+      <c r="G1" t="str">
+        <f>CONCATENATE("values('",B:B,"','",A:A,"','",B:B,"','",C:C,"','",D:D,"','admin',now());")</f>
+        <v>values('BAGS','BAG','BAGS','QTY','0','admin',now());</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="B2" t="s">
+        <v>98</v>
+      </c>
+      <c r="C2" t="s">
+        <v>95</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="F2" t="s">
+        <v>96</v>
+      </c>
+      <c r="G2" t="str">
+        <f t="shared" ref="G2:G44" si="0">CONCATENATE("values('",B:B,"','",A:A,"','",B:B,"','",C:C,"','",D:D,"','admin',now());")</f>
+        <v>values('BALE','BAL','BALE','QTY','0','admin',now());</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="B3" t="s">
+        <v>100</v>
+      </c>
+      <c r="C3" t="s">
+        <v>95</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="F3" t="s">
+        <v>96</v>
+      </c>
+      <c r="G3" t="str">
+        <f t="shared" si="0"/>
+        <v>values('BUNDLES','BDL','BUNDLES','QTY','0','admin',now());</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="B4" t="s">
+        <v>102</v>
+      </c>
+      <c r="C4" t="s">
+        <v>95</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="F4" t="s">
+        <v>96</v>
+      </c>
+      <c r="G4" t="str">
+        <f t="shared" si="0"/>
+        <v>values('BUCKLES','BKL','BUCKLES','QTY','0','admin',now());</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="B5" t="s">
+        <v>104</v>
+      </c>
+      <c r="C5" t="s">
+        <v>95</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="F5" t="s">
+        <v>96</v>
+      </c>
+      <c r="G5" t="str">
+        <f t="shared" si="0"/>
+        <v>values('BILLION OF UNITS','BOU','BILLION OF UNITS','QTY','0','admin',now());</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="B6" t="s">
+        <v>105</v>
+      </c>
+      <c r="C6" t="s">
+        <v>95</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="F6" t="s">
+        <v>96</v>
+      </c>
+      <c r="G6" t="str">
+        <f t="shared" si="0"/>
+        <v>values('BOX','BOX','BOX','QTY','0','admin',now());</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="B7" t="s">
+        <v>107</v>
+      </c>
+      <c r="C7" t="s">
+        <v>95</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="F7" t="s">
+        <v>96</v>
+      </c>
+      <c r="G7" t="str">
+        <f t="shared" si="0"/>
+        <v>values('BOTTLES','BTL','BOTTLES','QTY','0','admin',now());</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="B8" t="s">
+        <v>109</v>
+      </c>
+      <c r="C8" t="s">
+        <v>95</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="F8" t="s">
+        <v>96</v>
+      </c>
+      <c r="G8" t="str">
+        <f t="shared" si="0"/>
+        <v>values('BUNCHES','BUN','BUNCHES','QTY','0','admin',now());</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="B9" t="s">
+        <v>111</v>
+      </c>
+      <c r="C9" t="s">
+        <v>95</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="F9" t="s">
+        <v>96</v>
+      </c>
+      <c r="G9" t="str">
+        <f t="shared" si="0"/>
+        <v>values('CANS','CAN','CANS','QTY','0','admin',now());</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="B10" t="s">
+        <v>113</v>
+      </c>
+      <c r="C10" t="s">
+        <v>114</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="F10" t="s">
+        <v>96</v>
+      </c>
+      <c r="G10" t="str">
+        <f t="shared" si="0"/>
+        <v>values('CUBIC METERS','CBM','CUBIC METERS','VOLUME','0','admin',now());</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="B11" t="s">
+        <v>116</v>
+      </c>
+      <c r="C11" t="s">
+        <v>114</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="F11" t="s">
+        <v>96</v>
+      </c>
+      <c r="G11" t="str">
+        <f t="shared" si="0"/>
+        <v>values('CUBIC CENTIMETERS','CCM','CUBIC CENTIMETERS','VOLUME','0','admin',now());</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="B12" t="s">
+        <v>118</v>
+      </c>
+      <c r="C12" t="s">
+        <v>119</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="F12" t="s">
+        <v>96</v>
+      </c>
+      <c r="G12" t="str">
+        <f t="shared" si="0"/>
+        <v>values('CENTIMETERS','CMS','CENTIMETERS','LENGTH','0','admin',now());</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="B13" t="s">
+        <v>121</v>
+      </c>
+      <c r="C13" t="s">
+        <v>95</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="F13" t="s">
+        <v>96</v>
+      </c>
+      <c r="G13" t="str">
+        <f t="shared" si="0"/>
+        <v>values('CARTONS','CTN','CARTONS','QTY','0','admin',now());</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="B14" t="s">
+        <v>123</v>
+      </c>
+      <c r="C14" t="s">
+        <v>95</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+      <c r="F14" t="s">
+        <v>96</v>
+      </c>
+      <c r="G14" t="str">
+        <f t="shared" si="0"/>
+        <v>values('DOZENS','DOZ','DOZENS','QTY','0','admin',now());</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="8" t="s">
+        <v>124</v>
+      </c>
+      <c r="B15" t="s">
+        <v>125</v>
+      </c>
+      <c r="C15" t="s">
+        <v>95</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+      <c r="F15" t="s">
+        <v>96</v>
+      </c>
+      <c r="G15" t="str">
+        <f t="shared" si="0"/>
+        <v>values('DRUMS','DRM','DRUMS','QTY','0','admin',now());</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="8" t="s">
+        <v>126</v>
+      </c>
+      <c r="B16" t="s">
+        <v>127</v>
+      </c>
+      <c r="C16" t="s">
+        <v>95</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+      <c r="F16" t="s">
+        <v>96</v>
+      </c>
+      <c r="G16" t="str">
+        <f t="shared" si="0"/>
+        <v>values('GREAT GROSS','GGK','GREAT GROSS','QTY','0','admin',now());</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="8" t="s">
+        <v>128</v>
+      </c>
+      <c r="B17" t="s">
+        <v>129</v>
+      </c>
+      <c r="C17" t="s">
+        <v>130</v>
+      </c>
+      <c r="D17">
+        <v>0</v>
+      </c>
+      <c r="F17" t="s">
+        <v>96</v>
+      </c>
+      <c r="G17" t="str">
+        <f t="shared" si="0"/>
+        <v>values('GRAMMES','GMS','GRAMMES','WEIGHT','0','admin',now());</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="8" t="s">
+        <v>131</v>
+      </c>
+      <c r="B18" t="s">
+        <v>132</v>
+      </c>
+      <c r="C18" t="s">
+        <v>95</v>
+      </c>
+      <c r="D18">
+        <v>0</v>
+      </c>
+      <c r="F18" t="s">
+        <v>96</v>
+      </c>
+      <c r="G18" t="str">
+        <f t="shared" si="0"/>
+        <v>values('GROSS','GRS','GROSS','QTY','0','admin',now());</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="8" t="s">
+        <v>133</v>
+      </c>
+      <c r="B19" t="s">
+        <v>134</v>
+      </c>
+      <c r="C19" t="s">
+        <v>119</v>
+      </c>
+      <c r="D19">
+        <v>0</v>
+      </c>
+      <c r="F19" t="s">
+        <v>96</v>
+      </c>
+      <c r="G19" t="str">
+        <f t="shared" si="0"/>
+        <v>values('GROSS YARDS','GYD','GROSS YARDS','LENGTH','0','admin',now());</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="B20" t="s">
+        <v>136</v>
+      </c>
+      <c r="C20" t="s">
+        <v>130</v>
+      </c>
+      <c r="D20">
+        <v>1</v>
+      </c>
+      <c r="F20" t="s">
+        <v>96</v>
+      </c>
+      <c r="G20" t="str">
+        <f t="shared" si="0"/>
+        <v>values('KILOGRAMS','KGS','KILOGRAMS','WEIGHT','1','admin',now());</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="8" t="s">
+        <v>137</v>
+      </c>
+      <c r="B21" t="s">
+        <v>138</v>
+      </c>
+      <c r="C21" t="s">
+        <v>114</v>
+      </c>
+      <c r="D21">
+        <v>1</v>
+      </c>
+      <c r="F21" t="s">
+        <v>96</v>
+      </c>
+      <c r="G21" t="str">
+        <f t="shared" si="0"/>
+        <v>values('KILOLITRE','KLR','KILOLITRE','VOLUME','1','admin',now());</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="B22" t="s">
+        <v>140</v>
+      </c>
+      <c r="C22" t="s">
+        <v>119</v>
+      </c>
+      <c r="D22">
+        <v>0</v>
+      </c>
+      <c r="F22" t="s">
+        <v>96</v>
+      </c>
+      <c r="G22" t="str">
+        <f t="shared" si="0"/>
+        <v>values('KILOMETRE','KME','KILOMETRE','LENGTH','0','admin',now());</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="8" t="s">
+        <v>141</v>
+      </c>
+      <c r="B23" t="s">
+        <v>142</v>
+      </c>
+      <c r="C23" t="s">
+        <v>114</v>
+      </c>
+      <c r="D23">
+        <v>0</v>
+      </c>
+      <c r="F23" t="s">
+        <v>96</v>
+      </c>
+      <c r="G23" t="str">
+        <f t="shared" si="0"/>
+        <v>values('MILILITRE','MLT','MILILITRE','VOLUME','0','admin',now());</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="B24" t="s">
+        <v>144</v>
+      </c>
+      <c r="C24" t="s">
+        <v>119</v>
+      </c>
+      <c r="D24">
+        <v>1</v>
+      </c>
+      <c r="F24" t="s">
+        <v>96</v>
+      </c>
+      <c r="G24" t="str">
+        <f t="shared" si="0"/>
+        <v>values('METERS','MTR','METERS','LENGTH','1','admin',now());</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="B25" t="s">
+        <v>146</v>
+      </c>
+      <c r="C25" t="s">
+        <v>130</v>
+      </c>
+      <c r="D25">
+        <v>0</v>
+      </c>
+      <c r="F25" t="s">
+        <v>96</v>
+      </c>
+      <c r="G25" t="str">
+        <f t="shared" si="0"/>
+        <v>values('METRIC TON','MTS','METRIC TON','WEIGHT','0','admin',now());</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="8" t="s">
+        <v>147</v>
+      </c>
+      <c r="B26" t="s">
+        <v>148</v>
+      </c>
+      <c r="C26" t="s">
+        <v>95</v>
+      </c>
+      <c r="D26">
+        <v>1</v>
+      </c>
+      <c r="F26" t="s">
+        <v>96</v>
+      </c>
+      <c r="G26" t="str">
+        <f t="shared" si="0"/>
+        <v>values('NUMBERS','NOS','NUMBERS','QTY','1','admin',now());</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="8" t="s">
+        <v>149</v>
+      </c>
+      <c r="B27" t="s">
+        <v>150</v>
+      </c>
+      <c r="C27" t="s">
+        <v>95</v>
+      </c>
+      <c r="D27">
+        <v>0</v>
+      </c>
+      <c r="F27" t="s">
+        <v>96</v>
+      </c>
+      <c r="G27" t="str">
+        <f t="shared" si="0"/>
+        <v>values('PACKS','PAC','PACKS','QTY','0','admin',now());</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" s="8" t="s">
+        <v>151</v>
+      </c>
+      <c r="B28" t="s">
+        <v>152</v>
+      </c>
+      <c r="C28" t="s">
+        <v>95</v>
+      </c>
+      <c r="D28">
+        <v>0</v>
+      </c>
+      <c r="F28" t="s">
+        <v>96</v>
+      </c>
+      <c r="G28" t="str">
+        <f t="shared" si="0"/>
+        <v>values('PIECES','PCS','PIECES','QTY','0','admin',now());</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" s="8" t="s">
+        <v>153</v>
+      </c>
+      <c r="B29" t="s">
+        <v>154</v>
+      </c>
+      <c r="C29" t="s">
+        <v>95</v>
+      </c>
+      <c r="D29">
+        <v>0</v>
+      </c>
+      <c r="F29" t="s">
+        <v>96</v>
+      </c>
+      <c r="G29" t="str">
+        <f t="shared" si="0"/>
+        <v>values('PAIRS','PRS','PAIRS','QTY','0','admin',now());</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="B30" t="s">
+        <v>156</v>
+      </c>
+      <c r="C30" t="s">
+        <v>130</v>
+      </c>
+      <c r="D30">
+        <v>0</v>
+      </c>
+      <c r="F30" t="s">
+        <v>96</v>
+      </c>
+      <c r="G30" t="str">
+        <f t="shared" si="0"/>
+        <v>values('QUINTAL','QTL','QUINTAL','WEIGHT','0','admin',now());</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="B31" t="s">
+        <v>158</v>
+      </c>
+      <c r="C31" t="s">
+        <v>95</v>
+      </c>
+      <c r="D31">
+        <v>0</v>
+      </c>
+      <c r="F31" t="s">
+        <v>96</v>
+      </c>
+      <c r="G31" t="str">
+        <f t="shared" si="0"/>
+        <v>values('ROLLS','ROL','ROLLS','QTY','0','admin',now());</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" s="8" t="s">
+        <v>159</v>
+      </c>
+      <c r="B32" t="s">
+        <v>160</v>
+      </c>
+      <c r="C32" t="s">
+        <v>95</v>
+      </c>
+      <c r="D32">
+        <v>0</v>
+      </c>
+      <c r="F32" t="s">
+        <v>96</v>
+      </c>
+      <c r="G32" t="str">
+        <f t="shared" si="0"/>
+        <v>values('SETS','SET','SETS','QTY','0','admin',now());</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" s="8" t="s">
+        <v>161</v>
+      </c>
+      <c r="B33" t="s">
+        <v>162</v>
+      </c>
+      <c r="C33" t="s">
+        <v>163</v>
+      </c>
+      <c r="D33">
+        <v>1</v>
+      </c>
+      <c r="F33" t="s">
+        <v>96</v>
+      </c>
+      <c r="G33" t="str">
+        <f t="shared" si="0"/>
+        <v>values('SQUARE FEET','SQF','SQUARE FEET','AREA','1','admin',now());</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34" s="8" t="s">
+        <v>164</v>
+      </c>
+      <c r="B34" t="s">
+        <v>165</v>
+      </c>
+      <c r="C34" t="s">
+        <v>163</v>
+      </c>
+      <c r="D34">
+        <v>0</v>
+      </c>
+      <c r="F34" t="s">
+        <v>96</v>
+      </c>
+      <c r="G34" t="str">
+        <f t="shared" si="0"/>
+        <v>values('SQUARE METERS','SQM','SQUARE METERS','AREA','0','admin',now());</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35" s="8" t="s">
+        <v>166</v>
+      </c>
+      <c r="B35" t="s">
+        <v>167</v>
+      </c>
+      <c r="C35" t="s">
+        <v>163</v>
+      </c>
+      <c r="D35">
+        <v>0</v>
+      </c>
+      <c r="F35" t="s">
+        <v>96</v>
+      </c>
+      <c r="G35" t="str">
+        <f t="shared" si="0"/>
+        <v>values('SQUARE YARDS','SQY','SQUARE YARDS','AREA','0','admin',now());</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="B36" t="s">
+        <v>169</v>
+      </c>
+      <c r="C36" t="s">
+        <v>95</v>
+      </c>
+      <c r="D36">
+        <v>0</v>
+      </c>
+      <c r="F36" t="s">
+        <v>96</v>
+      </c>
+      <c r="G36" t="str">
+        <f t="shared" si="0"/>
+        <v>values('TABLETS','TBS','TABLETS','QTY','0','admin',now());</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37" s="8" t="s">
+        <v>170</v>
+      </c>
+      <c r="B37" t="s">
+        <v>171</v>
+      </c>
+      <c r="C37" t="s">
+        <v>95</v>
+      </c>
+      <c r="D37">
+        <v>0</v>
+      </c>
+      <c r="F37" t="s">
+        <v>96</v>
+      </c>
+      <c r="G37" t="str">
+        <f t="shared" si="0"/>
+        <v>values('TEN GROSS','TGM','TEN GROSS','QTY','0','admin',now());</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38" s="8" t="s">
+        <v>172</v>
+      </c>
+      <c r="B38" t="s">
+        <v>173</v>
+      </c>
+      <c r="C38" t="s">
+        <v>95</v>
+      </c>
+      <c r="D38">
+        <v>0</v>
+      </c>
+      <c r="F38" t="s">
+        <v>96</v>
+      </c>
+      <c r="G38" t="str">
+        <f t="shared" si="0"/>
+        <v>values('THOUSANDS','THD','THOUSANDS','QTY','0','admin',now());</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A39" s="8" t="s">
+        <v>174</v>
+      </c>
+      <c r="B39" t="s">
+        <v>175</v>
+      </c>
+      <c r="C39" t="s">
+        <v>130</v>
+      </c>
+      <c r="D39">
+        <v>0</v>
+      </c>
+      <c r="F39" t="s">
+        <v>96</v>
+      </c>
+      <c r="G39" t="str">
+        <f t="shared" si="0"/>
+        <v>values('TONNES','TON','TONNES','WEIGHT','0','admin',now());</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A40" s="8" t="s">
+        <v>176</v>
+      </c>
+      <c r="B40" t="s">
+        <v>177</v>
+      </c>
+      <c r="C40" t="s">
+        <v>130</v>
+      </c>
+      <c r="D40">
+        <v>0</v>
+      </c>
+      <c r="F40" t="s">
+        <v>96</v>
+      </c>
+      <c r="G40" t="str">
+        <f t="shared" si="0"/>
+        <v>values('TUBES','TUB','TUBES','WEIGHT','0','admin',now());</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A41" s="8" t="s">
+        <v>178</v>
+      </c>
+      <c r="B41" t="s">
+        <v>179</v>
+      </c>
+      <c r="C41" t="s">
+        <v>114</v>
+      </c>
+      <c r="D41">
+        <v>0</v>
+      </c>
+      <c r="F41" t="s">
+        <v>96</v>
+      </c>
+      <c r="G41" t="str">
+        <f t="shared" si="0"/>
+        <v>values('US GALLONS','UGS','US GALLONS','VOLUME','0','admin',now());</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A42" s="8" t="s">
+        <v>180</v>
+      </c>
+      <c r="B42" t="s">
+        <v>181</v>
+      </c>
+      <c r="C42" t="s">
+        <v>95</v>
+      </c>
+      <c r="D42">
+        <v>0</v>
+      </c>
+      <c r="F42" t="s">
+        <v>96</v>
+      </c>
+      <c r="G42" t="str">
+        <f t="shared" si="0"/>
+        <v>values('UNITS','UNT','UNITS','QTY','0','admin',now());</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A43" s="8" t="s">
+        <v>182</v>
+      </c>
+      <c r="B43" t="s">
+        <v>183</v>
+      </c>
+      <c r="C43" t="s">
+        <v>119</v>
+      </c>
+      <c r="D43">
+        <v>0</v>
+      </c>
+      <c r="F43" t="s">
+        <v>96</v>
+      </c>
+      <c r="G43" t="str">
+        <f t="shared" si="0"/>
+        <v>values('YARDS','YDS','YARDS','LENGTH','0','admin',now());</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A44" s="8" t="s">
+        <v>184</v>
+      </c>
+      <c r="B44" t="s">
+        <v>185</v>
+      </c>
+      <c r="C44" t="s">
+        <v>185</v>
+      </c>
+      <c r="D44">
+        <v>0</v>
+      </c>
+      <c r="F44" t="s">
+        <v>96</v>
+      </c>
+      <c r="G44" t="str">
+        <f t="shared" si="0"/>
+        <v>values('OTHERS','OTH','OTHERS','OTHERS','0','admin',now());</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>